<commit_message>
added new items to best solutions and guidelines
</commit_message>
<xml_diff>
--- a/src/assets/Data/BestPractices/Rapid Assessment Tool/FED Rapid Assessment Tool.xlsx
+++ b/src/assets/Data/BestPractices/Rapid Assessment Tool/FED Rapid Assessment Tool.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - LTI\OneDrive for~1\FED related items\Rapid Rollout Framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lntinfotech.sharepoint.com/sites/FEDAssetsInventory-RapidRolloutFramework/Shared Documents/Rapid Rollout Framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="8_{2B046B4A-CFED-4CEF-8763-E9554D20A205}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{AC84A497-6973-4FC2-A226-70EC95435BDA}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{2B046B4A-CFED-4CEF-8763-E9554D20A205}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{FD5BC20C-E541-4272-8CAC-11BE60098589}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{29329CCC-968E-4CDD-97C9-29D750550FFD}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Featured Queries " sheetId="4" r:id="rId3"/>
     <sheet name="Guidance" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,108 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
   <si>
     <t>Features</t>
-  </si>
-  <si>
-    <t>User Experience</t>
-  </si>
-  <si>
-    <t>Ease of Use</t>
-  </si>
-  <si>
-    <t>Visual Appeal</t>
-  </si>
-  <si>
-    <t>Accessibility</t>
-  </si>
-  <si>
-    <t>Navigation</t>
-  </si>
-  <si>
-    <t>Responsiveness</t>
-  </si>
-  <si>
-    <t>Current State</t>
-  </si>
-  <si>
-    <t>Aspiration</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>SQL Injection</t>
-  </si>
-  <si>
-    <t>Cross Site scripting</t>
-  </si>
-  <si>
-    <t>Remote File Inclusion</t>
-  </si>
-  <si>
-    <t>Cross site request Forgery</t>
-  </si>
-  <si>
-    <t>HTTPS</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Continuous Integration</t>
-  </si>
-  <si>
-    <t>Continuous Deployment</t>
-  </si>
-  <si>
-    <t>Automated Code review</t>
-  </si>
-  <si>
-    <t>Performance</t>
-  </si>
-  <si>
-    <t>Omnichannel Access</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Business Readiness</t>
-  </si>
-  <si>
-    <t>Page Load time</t>
-  </si>
-  <si>
-    <t>Server Time</t>
-  </si>
-  <si>
-    <t>Time to Interact</t>
-  </si>
-  <si>
-    <t>Web access</t>
-  </si>
-  <si>
-    <t>Mobile access</t>
-  </si>
-  <si>
-    <t>Code reusability</t>
-  </si>
-  <si>
-    <t>Technology stack</t>
-  </si>
-  <si>
-    <t>Omnichannel</t>
-  </si>
-  <si>
-    <t>Search Engine Optimization</t>
   </si>
   <si>
     <r>
@@ -168,6 +69,45 @@
     </r>
   </si>
   <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>User Experience</t>
+  </si>
+  <si>
+    <t>Ease of Use</t>
+  </si>
+  <si>
+    <t>Visual Appeal</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>User Feedback / Survey</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>AI &amp; Chatbots</t>
+  </si>
+  <si>
+    <t>Push Notification</t>
+  </si>
+  <si>
+    <t>Voice Search</t>
+  </si>
+  <si>
+    <t>Search Engine Optimization</t>
+  </si>
+  <si>
+    <t>Responsiveness</t>
+  </si>
+  <si>
     <t>Screen size</t>
   </si>
   <si>
@@ -175,6 +115,279 @@
   </si>
   <si>
     <t>Orientation</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>SQL Injection</t>
+  </si>
+  <si>
+    <t>Cross Site scripting</t>
+  </si>
+  <si>
+    <t>Remote File Inclusion</t>
+  </si>
+  <si>
+    <t>Cross site request Forgery</t>
+  </si>
+  <si>
+    <t>Encryption</t>
+  </si>
+  <si>
+    <t>HTTPS</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Continuous Integration</t>
+  </si>
+  <si>
+    <t>Automated Test</t>
+  </si>
+  <si>
+    <t>Continuous Deployment</t>
+  </si>
+  <si>
+    <t>Automated Code review</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Page Load time</t>
+  </si>
+  <si>
+    <t>Server Time</t>
+  </si>
+  <si>
+    <t>Time to Interact</t>
+  </si>
+  <si>
+    <t>Omnichannel Access</t>
+  </si>
+  <si>
+    <t>Web access</t>
+  </si>
+  <si>
+    <t>Mobile access</t>
+  </si>
+  <si>
+    <t>Offline access</t>
+  </si>
+  <si>
+    <t>Technology/ Architecture</t>
+  </si>
+  <si>
+    <t>Technology stack</t>
+  </si>
+  <si>
+    <t>Microfrontends</t>
+  </si>
+  <si>
+    <t>Atomic Design</t>
+  </si>
+  <si>
+    <t>WebComps</t>
+  </si>
+  <si>
+    <t>RAIL</t>
+  </si>
+  <si>
+    <t>PWA</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>API Gateway / ESB</t>
+  </si>
+  <si>
+    <t>Microservices</t>
+  </si>
+  <si>
+    <t>Authentication / Authorization</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>Code reusability</t>
+  </si>
+  <si>
+    <t>Architectural document</t>
+  </si>
+  <si>
+    <t>Business Readiness</t>
+  </si>
+  <si>
+    <t>Requirement detailing</t>
+  </si>
+  <si>
+    <t>Current State</t>
+  </si>
+  <si>
+    <t>Aspiration</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ease of use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - How easy it is for a user to use the website; how easily a task can be completed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Visual Appeal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - How striking is the UI; does it appeal to explore a certain feature due to an impressive UI
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Accessibility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - How easy and flexible are the elements of a site designed to improve the ability of people with disabilities to independently use it
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Chat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- Feature where either a chatbot or an online executive is available to resolve user's issue
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Feedback/ Survey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Ability to take user feedback or survey
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Navigation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Ability to check how someone moves around on your website. An organized and transparent navigation system acts as a road map to direct visitors to various pages and information on your site.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SEO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Search engine bots indexs your website efficiently when they crawl your web pages. This is helpful to the website to be search by anyone using popular search site such as google</t>
+    </r>
+  </si>
+  <si>
+    <t>0: Not Considered
+1: Getting Started
+2: Developing
+3: Practicing
+4: Optimizing
+5: Transforming</t>
   </si>
   <si>
     <r>
@@ -239,166 +452,6 @@
     </r>
   </si>
   <si>
-    <t>Automated Test</t>
-  </si>
-  <si>
-    <t>Offline access</t>
-  </si>
-  <si>
-    <t>Chat</t>
-  </si>
-  <si>
-    <t>User Feedback / Survey</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ease of use</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - How easy it is for a user to use the website; how easily a task can be completed
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Visual Appeal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - How striking is the UI; does it appeal to explore a certain feature due to an impressive UI
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Accessibility</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - How easy and flexible are the elements of a site designed to improve the ability of people with disabilities to independently use it
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Chat </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Feature where either a chatbot or an online executive is available to resolve user's issue
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Feedback/ Survey</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Ability to take user feedback or survey
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Navigation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Ability to check how someone moves around on your website. An organized and transparent navigation system acts as a road map to direct visitors to various pages and information on your site.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>SEO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Search engine bots indexs your website efficiently when they crawl your web pages. This is helpful to the website to be search by anyone using popular search site such as google</t>
-    </r>
-  </si>
-  <si>
-    <t>Encryption</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -663,10 +716,15 @@
     </r>
   </si>
   <si>
-    <t>Requirement detailing</t>
-  </si>
-  <si>
-    <t>Architectural document</t>
+    <t>Omnichannel</t>
+  </si>
+  <si>
+    <t>Web Access - Is the portal accessible through all web browser 
+Mobile access - Is the portal accessible through mobile browser
+Offline access - Is the Portal available for offline usage</t>
+  </si>
+  <si>
+    <t>Technology</t>
   </si>
   <si>
     <r>
@@ -732,11 +790,6 @@
     </r>
   </si>
   <si>
-    <t>Web Access - Is the portal accessible through all web browser 
-Mobile access - Is the portal accessible through mobile browser
-Offline access - Is the Portal available for offline usage</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -758,51 +811,6 @@
       <t xml:space="preserve"> - How and what amount of requirement detailing is available and in what format
 </t>
     </r>
-  </si>
-  <si>
-    <t>Voice Search</t>
-  </si>
-  <si>
-    <t>Technology/ Architecture</t>
-  </si>
-  <si>
-    <t>Microfrontends</t>
-  </si>
-  <si>
-    <t>Atomic Design</t>
-  </si>
-  <si>
-    <t>WebComps</t>
-  </si>
-  <si>
-    <t>RAIL</t>
-  </si>
-  <si>
-    <t>PWA</t>
-  </si>
-  <si>
-    <t>AMP</t>
-  </si>
-  <si>
-    <t>AI &amp; Chatbots</t>
-  </si>
-  <si>
-    <t>Push Notification</t>
-  </si>
-  <si>
-    <t>API Gateway / ESB</t>
-  </si>
-  <si>
-    <t>Microservices</t>
-  </si>
-  <si>
-    <t>Authentication / Authorization</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>Questions</t>
   </si>
 </sst>
 </file>
@@ -1241,12 +1249,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1257,32 +1259,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1291,37 +1275,61 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4094,7 +4102,7 @@
   <dimension ref="A2:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4111,18 +4119,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="32">
         <f>SUM(C4:C13)/COUNTIF(C4:C13,"&gt;0")</f>
@@ -4137,7 +4145,7 @@
     <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -4150,7 +4158,7 @@
     <row r="5" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7">
         <v>2</v>
@@ -4163,7 +4171,7 @@
     <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -4176,7 +4184,7 @@
     <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
@@ -4189,7 +4197,7 @@
     <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="7" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C8" s="7">
         <v>2</v>
@@ -4202,7 +4210,7 @@
     <row r="9" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C9" s="7">
         <v>2.5</v>
@@ -4215,7 +4223,7 @@
     <row r="10" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="7" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -4228,7 +4236,7 @@
     <row r="11" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -4241,7 +4249,7 @@
     <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="7" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
@@ -4254,7 +4262,7 @@
     <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
@@ -4267,7 +4275,7 @@
     <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C15" s="33">
         <f>SUM(C16:C18)/COUNTIF(C16:C18,"&gt;0")</f>
@@ -4282,7 +4290,7 @@
     <row r="16" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="8" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C16" s="11">
         <v>3</v>
@@ -4295,7 +4303,7 @@
     <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="8" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C17" s="11">
         <v>3</v>
@@ -4308,7 +4316,7 @@
     <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="8" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C18" s="11">
         <v>2</v>
@@ -4321,7 +4329,7 @@
     <row r="19" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C20" s="34">
         <f>SUM(C21:C26)/COUNTIF(C21:C26,"&gt;0")</f>
@@ -4336,7 +4344,7 @@
     <row r="21" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C21" s="15">
         <v>0</v>
@@ -4349,7 +4357,7 @@
     <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C22" s="15">
         <v>0</v>
@@ -4362,7 +4370,7 @@
     <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C23" s="15">
         <v>0</v>
@@ -4375,7 +4383,7 @@
     <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="15" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C24" s="15">
         <v>0</v>
@@ -4388,7 +4396,7 @@
     <row r="25" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="15" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
@@ -4401,7 +4409,7 @@
     <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="15" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C26" s="15">
         <v>1</v>
@@ -4414,7 +4422,7 @@
     <row r="27" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="16" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C28" s="37">
         <f>IFERROR(SUM(C29:C32)/COUNTIF(C29:C32,"&gt;0"),0)</f>
@@ -4429,7 +4437,7 @@
     <row r="29" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="18" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C29" s="17">
         <v>0</v>
@@ -4442,7 +4450,7 @@
     <row r="30" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="18" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C30" s="17">
         <v>0</v>
@@ -4455,7 +4463,7 @@
     <row r="31" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="17" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C31" s="17">
         <v>0</v>
@@ -4468,7 +4476,7 @@
     <row r="32" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="17" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C32" s="17">
         <v>0</v>
@@ -4481,7 +4489,7 @@
     <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="20" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C34" s="38">
         <f>SUM(C35:C37)/COUNTIF(C35:C37,"&gt;0")</f>
@@ -4496,7 +4504,7 @@
     <row r="35" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="22" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C35" s="21">
         <v>3</v>
@@ -4509,7 +4517,7 @@
     <row r="36" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="22" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C36" s="21">
         <v>3</v>
@@ -4522,7 +4530,7 @@
     <row r="37" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="22" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C37" s="21">
         <v>3</v>
@@ -4535,7 +4543,7 @@
     <row r="38" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C39" s="41">
         <f>SUM(C40:C42)/COUNTIF(C40:C42,"&gt;0")</f>
@@ -4550,7 +4558,7 @@
     <row r="40" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="25" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C40" s="24">
         <v>1</v>
@@ -4563,7 +4571,7 @@
     <row r="41" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="25" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C41" s="24">
         <v>0</v>
@@ -4576,7 +4584,7 @@
     <row r="42" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C42" s="24">
         <v>1</v>
@@ -4589,7 +4597,7 @@
     <row r="43" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="26" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C44" s="39">
         <f>SUM(C45:C57)/COUNTIF(C45:C57,"&gt;0")</f>
@@ -4604,7 +4612,7 @@
     <row r="45" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="28" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C45" s="27">
         <v>2</v>
@@ -4617,7 +4625,7 @@
     <row r="46" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="28" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C46" s="27">
         <v>0</v>
@@ -4630,7 +4638,7 @@
     <row r="47" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="28" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C47" s="27">
         <v>0</v>
@@ -4643,7 +4651,7 @@
     <row r="48" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="28" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C48" s="27">
         <v>0</v>
@@ -4656,7 +4664,7 @@
     <row r="49" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="28" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C49" s="27">
         <v>0</v>
@@ -4669,7 +4677,7 @@
     <row r="50" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="28" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C50" s="27">
         <v>0</v>
@@ -4682,7 +4690,7 @@
     <row r="51" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="28" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C51" s="27">
         <v>0</v>
@@ -4695,7 +4703,7 @@
     <row r="52" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="28" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C52" s="27">
         <v>3</v>
@@ -4708,7 +4716,7 @@
     <row r="53" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="28" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C53" s="27">
         <v>3</v>
@@ -4721,7 +4729,7 @@
     <row r="54" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="28" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C54" s="27">
         <v>3</v>
@@ -4734,7 +4742,7 @@
     <row r="55" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="28" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C55" s="27">
         <v>2</v>
@@ -4747,7 +4755,7 @@
     <row r="56" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="28" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C56" s="27">
         <v>2</v>
@@ -4760,7 +4768,7 @@
     <row r="57" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C57" s="27">
         <v>1</v>
@@ -4773,7 +4781,7 @@
     <row r="58" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="29" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C59" s="40">
         <f>SUM(C60)/COUNTIF(C60,"&gt;0")</f>
@@ -4788,7 +4796,7 @@
     <row r="60" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="31" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C60" s="30">
         <v>2</v>
@@ -4825,10 +4833,10 @@
         <v>0</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="14:17" x14ac:dyDescent="0.25">
@@ -4970,342 +4978,342 @@
         <v>0</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="53"/>
+      <c r="B3" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="78"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="55"/>
+      <c r="B4" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="53"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="55"/>
+      <c r="B5" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="53"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="55"/>
+      <c r="B6" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="53"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="53"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="53"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="53"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="53"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="53"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="53"/>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="56"/>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="79" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="80"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="53"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="53"/>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="56"/>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="82"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="53"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="53"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="53"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="53"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="53"/>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="56"/>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="84"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="53"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="53"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="53"/>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="56"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="86"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="53"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="53"/>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="56"/>
+    </row>
+    <row r="38" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+    </row>
+    <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="87" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="88"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="53"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="53"/>
+    </row>
+    <row r="42" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="56"/>
+    </row>
+    <row r="43" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+    </row>
+    <row r="44" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="74"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="53"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="53"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="55"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="56" t="s">
+      <c r="C47" s="53"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="55"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="55"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="55"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="55"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="56" t="s">
+      <c r="C48" s="53"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="53"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="53"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="53"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="53"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="53"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="53"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="53"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="53"/>
+    </row>
+    <row r="57" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="56"/>
+    </row>
+    <row r="58" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+    </row>
+    <row r="59" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="76"/>
+    </row>
+    <row r="60" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="55"/>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="58"/>
-    </row>
-    <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-    </row>
-    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="61"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="55"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="55"/>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="58"/>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="65"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="55"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="66" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="55"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="55"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="55"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="55"/>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="58"/>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-    </row>
-    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="70"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="55"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="55"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="55"/>
-    </row>
-    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="58"/>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-    </row>
-    <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="75"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="76" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="55"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="76" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="55"/>
-    </row>
-    <row r="37" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="58"/>
-    </row>
-    <row r="38" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-    </row>
-    <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="79"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="55"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="55"/>
-    </row>
-    <row r="42" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="58"/>
-    </row>
-    <row r="43" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-    </row>
-    <row r="44" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="82" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="83"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="84" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="55"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="84" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="55"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="55"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="55"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="84" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" s="55"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="84" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="55"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="55"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="84" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="55"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="55"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="84" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="55"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" s="55"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="55"/>
-    </row>
-    <row r="57" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="85" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="58"/>
-    </row>
-    <row r="58" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
-    </row>
-    <row r="59" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="87"/>
-    </row>
-    <row r="60" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="58"/>
+      <c r="C60" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5327,7 +5335,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5335,7 +5343,7 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="94.140625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5346,24 +5354,26 @@
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="36" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="219" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="217.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
@@ -5374,7 +5384,7 @@
     <row r="6" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="9"/>
@@ -5382,10 +5392,12 @@
     <row r="7" spans="1:4" ht="78.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="11" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
@@ -5396,7 +5408,7 @@
     <row r="9" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="13"/>
@@ -5404,10 +5416,12 @@
     <row r="10" spans="1:4" ht="257.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="15" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C10" s="12"/>
-      <c r="D10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
@@ -5418,7 +5432,7 @@
     <row r="12" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="16" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="16"/>
@@ -5426,10 +5440,12 @@
     <row r="13" spans="1:4" ht="142.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="17" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
@@ -5440,7 +5456,7 @@
     <row r="15" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="20" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -5448,10 +5464,12 @@
     <row r="16" spans="1:4" ht="104.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
       <c r="B16" s="21" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="21" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
@@ -5462,18 +5480,20 @@
     <row r="18" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
       <c r="B18" s="23" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
     </row>
-    <row r="19" spans="1:4" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="78.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
       <c r="B19" s="24" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="D19" s="24" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
@@ -5484,7 +5504,7 @@
     <row r="21" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="26" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
@@ -5492,10 +5512,12 @@
     <row r="22" spans="1:4" ht="104.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="27" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
+      <c r="D22" s="27" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
@@ -5506,18 +5528,20 @@
     <row r="24" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24" s="29" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
     </row>
-    <row r="25" spans="1:4" ht="40.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="78.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25" s="30" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="D25" s="30" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -5527,44 +5551,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006DD3A7BF4F4A6540902CF577056B1E29" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bffbd341d1aeff83497c241122f56a79">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="93559f80-2e2e-4d74-911d-dbee0f10c222" xmlns:ns4="a9909da8-a943-46b9-b5a9-5a08acf910d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05001036160325035e32640e0be2fc3b" ns3:_="" ns4:_="">
-    <xsd:import namespace="93559f80-2e2e-4d74-911d-dbee0f10c222"/>
-    <xsd:import namespace="a9909da8-a943-46b9-b5a9-5a08acf910d7"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010092F1B0DF7838A341A8374181D606D5D2" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efa4420f8cb36698032089c4779ae3bf">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1202df35-0811-42f5-bbc3-d91f31d64ae4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf91d6f700cf070ed757fdfd618445a5" ns2:_="">
+    <xsd:import namespace="1202df35-0811-42f5-bbc3-d91f31d64ae4"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5572,27 +5576,29 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="93559f80-2e2e-4d74-911d-dbee0f10c222" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1202df35-0811-42f5-bbc3-d91f31d64ae4" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
@@ -5605,61 +5611,19 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a9909da8-a943-46b9-b5a9-5a08acf910d7" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="20" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -5764,19 +5728,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A7D2213-46A2-4112-AAF9-45974CF670EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{566B1468-014F-42A0-AEB2-82D8DE99348B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1202df35-0811-42f5-bbc3-d91f31d64ae4"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a9909da8-a943-46b9-b5a9-5a08acf910d7"/>
-    <ds:schemaRef ds:uri="93559f80-2e2e-4d74-911d-dbee0f10c222"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5790,20 +5770,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35E372FE-F100-478C-9712-6D5409605413}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A7D2213-46A2-4112-AAF9-45974CF670EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="93559f80-2e2e-4d74-911d-dbee0f10c222"/>
-    <ds:schemaRef ds:uri="a9909da8-a943-46b9-b5a9-5a08acf910d7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="1202df35-0811-42f5-bbc3-d91f31d64ae4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>